<commit_message>
adam opt based learning rates
</commit_message>
<xml_diff>
--- a/chatbotp3r3/eloss3and4levelNet.xlsx
+++ b/chatbotp3r3/eloss3and4levelNet.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="4">
   <si>
     <t>Epoch</t>
   </si>
@@ -33,6 +33,9 @@
   </si>
   <si>
     <t>Loss 4L</t>
+  </si>
+  <si>
+    <t>Diff</t>
   </si>
 </sst>
 </file>
@@ -846,63 +849,12 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="log"/>
-            <c:forward val="100"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-8.3076085120596374E-2"/>
-                  <c:y val="2.4315097867668504E-2"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
-                </a:p>
-              </c:txPr>
-            </c:trendlineLbl>
-          </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$108</c:f>
+              <c:f>Sheet1!$A$2:$A$138</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="107"/>
+                <c:ptCount val="137"/>
                 <c:pt idx="0">
                   <c:v>0.4</c:v>
                 </c:pt>
@@ -1139,16 +1091,166 @@
                 </c:pt>
                 <c:pt idx="78">
                   <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>77</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>79</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>81</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>82</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>83</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>84</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>86</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>87</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>88</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>89</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>91</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>99</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>101</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>102</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>103</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>104</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>105</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>106</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>107</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>108</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>109</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>111</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>112</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>113</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>114</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>115</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>116</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>117</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>118</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>119</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>121</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>122</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>123</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$108</c:f>
+              <c:f>Sheet1!$B$2:$B$138</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="107"/>
+                <c:ptCount val="137"/>
                 <c:pt idx="0">
                   <c:v>4.1950000000000003</c:v>
                 </c:pt>
@@ -1385,6 +1487,132 @@
                 </c:pt>
                 <c:pt idx="78">
                   <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>1.391</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>1.389</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>1.391</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>1.38</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>1.3720000000000001</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>1.3660000000000001</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>1.369</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>1.367</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>1.3540000000000001</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>1.3560000000000001</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>1.351</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>1.3480000000000001</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>1.347</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>1.347</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>1.3380000000000001</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>1.333</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>1.3360000000000001</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>1.335</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>1.331</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>1.3260000000000001</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>1.3220000000000001</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>1.323</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>1.3169999999999999</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>1.3140000000000001</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>1.3129999999999999</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>1.3140000000000001</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>1.3049999999999999</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>1.3</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>1.296</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>1.2909999999999999</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>1.298</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>1.2949999999999999</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>1.2909999999999999</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>1.2849999999999999</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>1.284</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>1.2849999999999999</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>1.274</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>1.2789999999999999</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>1.2789999999999999</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>1.2769999999999999</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>1.27</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>1.272</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1432,63 +1660,12 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="log"/>
-            <c:forward val="40"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-4.4845831364354945E-2"/>
-                  <c:y val="-6.7440099399339787E-2"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
-                </a:p>
-              </c:txPr>
-            </c:trendlineLbl>
-          </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$D$108</c:f>
+              <c:f>Sheet1!$D$2:$D$157</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="107"/>
+                <c:ptCount val="156"/>
                 <c:pt idx="0">
                   <c:v>0.1</c:v>
                 </c:pt>
@@ -1809,16 +1986,163 @@
                 </c:pt>
                 <c:pt idx="106">
                   <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>111</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>112</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>113</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>114</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>115</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>116</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>117</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>118</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>119</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>121</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>122</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>123</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>124</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>126</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>127</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>129</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>131</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>132</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>133</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>134</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>135</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>136</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>137</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>138</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>139</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>141</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>142</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>143</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>144</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>145</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>146</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>147</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>148</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>149</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>151</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>152</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>153</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>154</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>155</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>156</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>157</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>158</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>159</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$E$2:$E$108</c:f>
+              <c:f>Sheet1!$E$2:$E$157</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="107"/>
+                <c:ptCount val="156"/>
                 <c:pt idx="0">
                   <c:v>5.5010000000000003</c:v>
                 </c:pt>
@@ -2139,6 +2463,153 @@
                 </c:pt>
                 <c:pt idx="106">
                   <c:v>1.431</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>1.3740000000000001</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>1.3640000000000001</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>1.369</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>1.357</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>1.355</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>1.355</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>1.3540000000000001</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>1.3480000000000001</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>1.343</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>1.347</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>1.335</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>1.3420000000000001</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>1.3340000000000001</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>1.3280000000000001</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>1.33</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>1.323</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>1.32</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>1.323</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>1.3169999999999999</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>1.3120000000000001</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>1.3089999999999999</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>1.306</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>1.298</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>1.304</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>1.2949999999999999</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>1.302</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>1.298</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>1.2969999999999999</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>1.2929999999999999</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>1.282</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>1.2809999999999999</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>1.2849999999999999</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>1.282</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>1.2789999999999999</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>1.2649999999999999</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>1.268</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>1.2709999999999999</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>1.27</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>1.2649999999999999</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>1.27</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>1.2629999999999999</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>1.262</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>1.254</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>1.2509999999999999</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>1.254</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>1.254</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>1.2490000000000001</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>1.246</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>1.25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2282,6 +2753,7 @@
         <c:axId val="474994784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="1"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -2471,6 +2943,971 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Diff</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$2:$D$113</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="112"/>
+                <c:pt idx="0">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>61</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>67</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>69</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>77</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>79</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>81</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>82</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>83</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>84</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>86</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>87</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>88</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>89</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>91</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>111</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>112</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>113</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>114</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>115</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$F$2:$F$113</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="112"/>
+                <c:pt idx="0">
+                  <c:v>-1.306</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-0.74299999999999944</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-0.47399999999999975</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-0.34699999999999953</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-0.2629999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-0.28000000000000025</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-0.27400000000000002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-0.41199999999999992</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-0.58400000000000007</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-0.7200000000000002</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-0.68800000000000017</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-0.62200000000000033</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-0.59299999999999997</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-0.58899999999999997</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-0.5860000000000003</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-0.59199999999999964</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-0.59399999999999986</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>-0.59799999999999986</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>-0.61499999999999977</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>-0.62199999999999989</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>-0.621</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>-0.60499999999999998</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>-0.6080000000000001</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>-0.59999999999999964</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>-0.59799999999999986</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>-0.59600000000000009</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>-0.58399999999999985</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>-0.58599999999999985</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>-0.57099999999999995</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>-0.56299999999999994</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>-0.55699999999999994</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>-0.54399999999999982</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>-0.53000000000000025</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>-0.53399999999999981</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>-0.51200000000000001</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>-0.5</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>-0.50299999999999989</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>-0.49</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>-0.47899999999999987</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>-0.47499999999999987</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>-0.46299999999999986</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>-0.44900000000000007</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>-0.44600000000000017</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>-0.43199999999999994</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>-0.41899999999999982</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>-0.41099999999999981</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>-0.41299999999999981</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>-0.39999999999999991</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>-0.39100000000000001</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>-0.38500000000000001</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>-0.375</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>-0.37199999999999989</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>-0.3640000000000001</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>-0.34800000000000009</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>-0.34200000000000008</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>-0.33100000000000018</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>-0.33200000000000007</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>-0.30400000000000005</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>-0.31600000000000006</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>-0.30899999999999994</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>-0.29499999999999993</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>-0.29499999999999993</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>-0.28599999999999981</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>-0.28399999999999981</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>-0.27600000000000002</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>-0.27</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>-0.26400000000000001</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>-0.26400000000000001</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>-0.25099999999999989</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>-0.2370000000000001</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>-0.24299999999999988</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>-0.23799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>-0.23299999999999987</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>-0.23799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>-0.21999999999999997</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>-0.22300000000000009</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>-0.21100000000000008</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>-0.20500000000000007</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>-0.20300000000000007</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>-0.21199999999999997</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>-0.19900000000000007</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>-0.18599999999999994</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>-0.19000000000000017</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>-0.19699999999999984</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>-0.18999999999999995</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>-0.17599999999999993</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>-0.17199999999999993</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>-0.18099999999999983</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>-0.16899999999999982</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>-0.16799999999999993</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>-0.16599999999999993</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>-0.16500000000000004</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>-0.15500000000000003</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>-0.16699999999999982</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>-0.16000000000000014</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>-0.1419999999999999</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>-0.14500000000000002</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>-0.14700000000000002</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>-0.14300000000000002</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>-0.14300000000000002</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>-0.13800000000000012</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>-0.13700000000000001</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>-0.13700000000000001</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>-0.129</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>-0.12199999999999989</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>-0.13100000000000001</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>-0.13100000000000001</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>-7.8000000000000069E-2</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>-7.3000000000000176E-2</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>-7.0999999999999952E-2</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>-6.2000000000000055E-2</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>-6.4000000000000057E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-A7E7-457E-9F48-09B96029BE0A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="474593584"/>
+        <c:axId val="449905792"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="474593584"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="449905792"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="449905792"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="474593584"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -2551,6 +3988,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -3583,20 +5060,536 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>285750</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>80010</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>377190</xdr:colOff>
-      <xdr:row>58</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>259080</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>49530</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3623,16 +5616,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>476250</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>106680</xdr:rowOff>
+      <xdr:rowOff>41910</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>624840</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>243840</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>163830</xdr:rowOff>
+      <xdr:rowOff>99060</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3654,6 +5647,44 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>83820</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>80010</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AEB2D331-E5D5-456B-8F30-A5978F6F9639}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3959,15 +5990,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E108"/>
+  <dimension ref="A1:F160"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C80"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3980,8 +6011,11 @@
       <c r="E1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A2">
         <v>0.4</v>
       </c>
@@ -3997,8 +6031,12 @@
       <c r="E2">
         <v>5.5010000000000003</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F2">
+        <f>B2-E2</f>
+        <v>-1.306</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A3">
         <v>0.5</v>
       </c>
@@ -4014,8 +6052,12 @@
       <c r="E3">
         <v>4.84</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F3">
+        <f t="shared" ref="F3:F66" si="0">B3-E3</f>
+        <v>-0.74299999999999944</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A4">
         <v>0.6</v>
       </c>
@@ -4031,8 +6073,12 @@
       <c r="E4">
         <v>4.4669999999999996</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F4">
+        <f t="shared" si="0"/>
+        <v>-0.47399999999999975</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A5">
         <v>0.7</v>
       </c>
@@ -4048,8 +6094,12 @@
       <c r="E5">
         <v>4.2809999999999997</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>-0.34699999999999953</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A6">
         <v>0.8</v>
       </c>
@@ -4065,8 +6115,12 @@
       <c r="E6">
         <v>4.1459999999999999</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>-0.2629999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A7">
         <v>0.9</v>
       </c>
@@ -4082,8 +6136,12 @@
       <c r="E7">
         <v>4.0880000000000001</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>-0.28000000000000025</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A8">
         <v>1</v>
       </c>
@@ -4099,8 +6157,12 @@
       <c r="E8">
         <v>4.032</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>-0.27400000000000002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A9">
         <v>2</v>
       </c>
@@ -4116,8 +6178,12 @@
       <c r="E9">
         <v>3.9889999999999999</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>-0.41199999999999992</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A10">
         <v>3</v>
       </c>
@@ -4133,8 +6199,12 @@
       <c r="E10">
         <v>3.9550000000000001</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>-0.58400000000000007</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A11">
         <v>4</v>
       </c>
@@ -4150,8 +6220,12 @@
       <c r="E11">
         <v>3.9390000000000001</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F11">
+        <f t="shared" si="0"/>
+        <v>-0.7200000000000002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A12">
         <v>5</v>
       </c>
@@ -4167,8 +6241,12 @@
       <c r="E12">
         <v>3.762</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>-0.68800000000000017</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A13">
         <v>6</v>
       </c>
@@ -4184,8 +6262,12 @@
       <c r="E13">
         <v>3.5670000000000002</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F13">
+        <f t="shared" si="0"/>
+        <v>-0.62200000000000033</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A14">
         <v>7</v>
       </c>
@@ -4201,8 +6283,12 @@
       <c r="E14">
         <v>3.43</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F14">
+        <f t="shared" si="0"/>
+        <v>-0.59299999999999997</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A15">
         <v>8</v>
       </c>
@@ -4218,8 +6304,12 @@
       <c r="E15">
         <v>3.32</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F15">
+        <f t="shared" si="0"/>
+        <v>-0.58899999999999997</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A16">
         <v>9</v>
       </c>
@@ -4235,8 +6325,12 @@
       <c r="E16">
         <v>3.2330000000000001</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F16">
+        <f t="shared" si="0"/>
+        <v>-0.5860000000000003</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A17">
         <v>10</v>
       </c>
@@ -4252,8 +6346,12 @@
       <c r="E17">
         <v>3.1469999999999998</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F17">
+        <f t="shared" si="0"/>
+        <v>-0.59199999999999964</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A18">
         <v>11</v>
       </c>
@@ -4269,8 +6367,12 @@
       <c r="E18">
         <v>3.08</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F18">
+        <f t="shared" si="0"/>
+        <v>-0.59399999999999986</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A19">
         <v>12</v>
       </c>
@@ -4286,8 +6388,12 @@
       <c r="E19">
         <v>3.008</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F19">
+        <f t="shared" si="0"/>
+        <v>-0.59799999999999986</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A20">
         <v>13</v>
       </c>
@@ -4303,8 +6409,12 @@
       <c r="E20">
         <v>2.9649999999999999</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F20">
+        <f t="shared" si="0"/>
+        <v>-0.61499999999999977</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A21">
         <v>14</v>
       </c>
@@ -4320,8 +6430,12 @@
       <c r="E21">
         <v>2.911</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F21">
+        <f t="shared" si="0"/>
+        <v>-0.62199999999999989</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A22">
         <v>15</v>
       </c>
@@ -4337,8 +6451,12 @@
       <c r="E22">
         <v>2.8570000000000002</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F22">
+        <f t="shared" si="0"/>
+        <v>-0.621</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A23">
         <v>16</v>
       </c>
@@ -4354,8 +6472,12 @@
       <c r="E23">
         <v>2.7919999999999998</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F23">
+        <f t="shared" si="0"/>
+        <v>-0.60499999999999998</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A24">
         <v>17</v>
       </c>
@@ -4371,8 +6493,12 @@
       <c r="E24">
         <v>2.7490000000000001</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F24">
+        <f t="shared" si="0"/>
+        <v>-0.6080000000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A25">
         <v>18</v>
       </c>
@@ -4388,8 +6514,12 @@
       <c r="E25">
         <v>2.7029999999999998</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F25">
+        <f t="shared" si="0"/>
+        <v>-0.59999999999999964</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A26">
         <v>19</v>
       </c>
@@ -4405,8 +6535,12 @@
       <c r="E26">
         <v>2.6619999999999999</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F26">
+        <f t="shared" si="0"/>
+        <v>-0.59799999999999986</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A27">
         <v>20</v>
       </c>
@@ -4422,8 +6556,12 @@
       <c r="E27">
         <v>2.6240000000000001</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F27">
+        <f t="shared" si="0"/>
+        <v>-0.59600000000000009</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A28">
         <v>21</v>
       </c>
@@ -4439,8 +6577,12 @@
       <c r="E28">
         <v>2.581</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F28">
+        <f t="shared" si="0"/>
+        <v>-0.58399999999999985</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A29">
         <v>22</v>
       </c>
@@ -4456,8 +6598,12 @@
       <c r="E29">
         <v>2.5449999999999999</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F29">
+        <f t="shared" si="0"/>
+        <v>-0.58599999999999985</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A30">
         <v>23</v>
       </c>
@@ -4473,8 +6619,12 @@
       <c r="E30">
         <v>2.5049999999999999</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F30">
+        <f t="shared" si="0"/>
+        <v>-0.57099999999999995</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A31">
         <v>24</v>
       </c>
@@ -4490,8 +6640,12 @@
       <c r="E31">
         <v>2.4649999999999999</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F31">
+        <f t="shared" si="0"/>
+        <v>-0.56299999999999994</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A32">
         <v>25</v>
       </c>
@@ -4507,8 +6661,12 @@
       <c r="E32">
         <v>2.431</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F32">
+        <f t="shared" si="0"/>
+        <v>-0.55699999999999994</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A33">
         <v>26</v>
       </c>
@@ -4524,8 +6682,12 @@
       <c r="E33">
         <v>2.4009999999999998</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F33">
+        <f t="shared" si="0"/>
+        <v>-0.54399999999999982</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A34">
         <v>27</v>
       </c>
@@ -4541,8 +6703,12 @@
       <c r="E34">
         <v>2.3650000000000002</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F34">
+        <f t="shared" si="0"/>
+        <v>-0.53000000000000025</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A35">
         <v>28</v>
       </c>
@@ -4558,8 +6724,12 @@
       <c r="E35">
         <v>2.34</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F35">
+        <f t="shared" si="0"/>
+        <v>-0.53399999999999981</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A36">
         <v>29</v>
       </c>
@@ -4575,8 +6745,12 @@
       <c r="E36">
         <v>2.302</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F36">
+        <f t="shared" si="0"/>
+        <v>-0.51200000000000001</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A37">
         <v>30</v>
       </c>
@@ -4592,8 +6766,12 @@
       <c r="E37">
         <v>2.2749999999999999</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F37">
+        <f t="shared" si="0"/>
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A38">
         <v>31</v>
       </c>
@@ -4609,8 +6787,12 @@
       <c r="E38">
         <v>2.2589999999999999</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F38">
+        <f t="shared" si="0"/>
+        <v>-0.50299999999999989</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A39">
         <v>32</v>
       </c>
@@ -4626,8 +6808,12 @@
       <c r="E39">
         <v>2.2250000000000001</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F39">
+        <f t="shared" si="0"/>
+        <v>-0.49</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A40">
         <v>33</v>
       </c>
@@ -4643,8 +6829,12 @@
       <c r="E40">
         <v>2.198</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F40">
+        <f t="shared" si="0"/>
+        <v>-0.47899999999999987</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A41">
         <v>34</v>
       </c>
@@ -4660,8 +6850,12 @@
       <c r="E41">
         <v>2.1789999999999998</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F41">
+        <f t="shared" si="0"/>
+        <v>-0.47499999999999987</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A42">
         <v>35</v>
       </c>
@@ -4677,8 +6871,12 @@
       <c r="E42">
         <v>2.1459999999999999</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F42">
+        <f t="shared" si="0"/>
+        <v>-0.46299999999999986</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A43">
         <v>36</v>
       </c>
@@ -4694,8 +6892,12 @@
       <c r="E43">
         <v>2.125</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F43">
+        <f t="shared" si="0"/>
+        <v>-0.44900000000000007</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A44">
         <v>37</v>
       </c>
@@ -4711,8 +6913,12 @@
       <c r="E44">
         <v>2.1110000000000002</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F44">
+        <f t="shared" si="0"/>
+        <v>-0.44600000000000017</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A45">
         <v>38</v>
       </c>
@@ -4728,8 +6934,12 @@
       <c r="E45">
         <v>2.0819999999999999</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F45">
+        <f t="shared" si="0"/>
+        <v>-0.43199999999999994</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A46">
         <v>39</v>
       </c>
@@ -4745,8 +6955,12 @@
       <c r="E46">
         <v>2.0539999999999998</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F46">
+        <f t="shared" si="0"/>
+        <v>-0.41899999999999982</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A47">
         <v>40</v>
       </c>
@@ -4762,8 +6976,12 @@
       <c r="E47">
         <v>2.0329999999999999</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F47">
+        <f t="shared" si="0"/>
+        <v>-0.41099999999999981</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A48">
         <v>41</v>
       </c>
@@ -4779,8 +6997,12 @@
       <c r="E48">
         <v>2.0259999999999998</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F48">
+        <f t="shared" si="0"/>
+        <v>-0.41299999999999981</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A49">
         <v>42</v>
       </c>
@@ -4796,8 +7018,12 @@
       <c r="E49">
         <v>2.008</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F49">
+        <f t="shared" si="0"/>
+        <v>-0.39999999999999991</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A50">
         <v>43</v>
       </c>
@@ -4813,8 +7039,12 @@
       <c r="E50">
         <v>1.976</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F50">
+        <f t="shared" si="0"/>
+        <v>-0.39100000000000001</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A51">
         <v>44</v>
       </c>
@@ -4830,8 +7060,12 @@
       <c r="E51">
         <v>1.9630000000000001</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F51">
+        <f t="shared" si="0"/>
+        <v>-0.38500000000000001</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A52">
         <v>45</v>
       </c>
@@ -4847,8 +7081,12 @@
       <c r="E52">
         <v>1.9419999999999999</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F52">
+        <f t="shared" si="0"/>
+        <v>-0.375</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A53">
         <v>46</v>
       </c>
@@ -4864,8 +7102,12 @@
       <c r="E53">
         <v>1.9319999999999999</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F53">
+        <f t="shared" si="0"/>
+        <v>-0.37199999999999989</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A54">
         <v>47</v>
       </c>
@@ -4881,8 +7123,12 @@
       <c r="E54">
         <v>1.909</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F54">
+        <f t="shared" si="0"/>
+        <v>-0.3640000000000001</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A55">
         <v>48</v>
       </c>
@@ -4898,8 +7144,12 @@
       <c r="E55">
         <v>1.891</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F55">
+        <f t="shared" si="0"/>
+        <v>-0.34800000000000009</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A56">
         <v>49</v>
       </c>
@@ -4915,8 +7165,12 @@
       <c r="E56">
         <v>1.87</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F56">
+        <f t="shared" si="0"/>
+        <v>-0.34200000000000008</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A57">
         <v>50</v>
       </c>
@@ -4932,8 +7186,12 @@
       <c r="E57">
         <v>1.86</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F57">
+        <f t="shared" si="0"/>
+        <v>-0.33100000000000018</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A58">
         <v>51</v>
       </c>
@@ -4949,8 +7207,12 @@
       <c r="E58">
         <v>1.849</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F58">
+        <f t="shared" si="0"/>
+        <v>-0.33200000000000007</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A59">
         <v>52</v>
       </c>
@@ -4966,8 +7228,12 @@
       <c r="E59">
         <v>1.825</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F59">
+        <f t="shared" si="0"/>
+        <v>-0.30400000000000005</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A60">
         <v>53</v>
       </c>
@@ -4983,8 +7249,12 @@
       <c r="E60">
         <v>1.821</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F60">
+        <f t="shared" si="0"/>
+        <v>-0.31600000000000006</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A61">
         <v>54</v>
       </c>
@@ -5000,8 +7270,12 @@
       <c r="E61">
         <v>1.8029999999999999</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F61">
+        <f t="shared" si="0"/>
+        <v>-0.30899999999999994</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A62">
         <v>55</v>
       </c>
@@ -5017,8 +7291,12 @@
       <c r="E62">
         <v>1.79</v>
       </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F62">
+        <f t="shared" si="0"/>
+        <v>-0.29499999999999993</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A63">
         <v>56</v>
       </c>
@@ -5034,8 +7312,12 @@
       <c r="E63">
         <v>1.778</v>
       </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F63">
+        <f t="shared" si="0"/>
+        <v>-0.29499999999999993</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A64">
         <v>57</v>
       </c>
@@ -5051,8 +7333,12 @@
       <c r="E64">
         <v>1.7669999999999999</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F64">
+        <f t="shared" si="0"/>
+        <v>-0.28599999999999981</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A65">
         <v>58</v>
       </c>
@@ -5068,8 +7354,12 @@
       <c r="E65">
         <v>1.7589999999999999</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F65">
+        <f t="shared" si="0"/>
+        <v>-0.28399999999999981</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A66">
         <v>59</v>
       </c>
@@ -5085,8 +7375,12 @@
       <c r="E66">
         <v>1.738</v>
       </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F66">
+        <f t="shared" si="0"/>
+        <v>-0.27600000000000002</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A67">
         <v>60</v>
       </c>
@@ -5102,8 +7396,12 @@
       <c r="E67">
         <v>1.726</v>
       </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F67">
+        <f t="shared" ref="F67:F121" si="1">B67-E67</f>
+        <v>-0.27</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A68">
         <v>61</v>
       </c>
@@ -5119,8 +7417,12 @@
       <c r="E68">
         <v>1.7210000000000001</v>
       </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F68">
+        <f t="shared" si="1"/>
+        <v>-0.26400000000000001</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A69">
         <v>62</v>
       </c>
@@ -5136,8 +7438,12 @@
       <c r="E69">
         <v>1.7050000000000001</v>
       </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F69">
+        <f t="shared" si="1"/>
+        <v>-0.26400000000000001</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A70">
         <v>63</v>
       </c>
@@ -5153,8 +7459,12 @@
       <c r="E70">
         <v>1.698</v>
       </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F70">
+        <f t="shared" si="1"/>
+        <v>-0.25099999999999989</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A71">
         <v>64</v>
       </c>
@@ -5170,8 +7480,12 @@
       <c r="E71">
         <v>1.681</v>
       </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F71">
+        <f t="shared" si="1"/>
+        <v>-0.2370000000000001</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A72">
         <v>65</v>
       </c>
@@ -5187,8 +7501,12 @@
       <c r="E72">
         <v>1.6819999999999999</v>
       </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F72">
+        <f t="shared" si="1"/>
+        <v>-0.24299999999999988</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A73">
         <v>66</v>
       </c>
@@ -5204,8 +7522,12 @@
       <c r="E73">
         <v>1.663</v>
       </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F73">
+        <f t="shared" si="1"/>
+        <v>-0.23799999999999999</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A74">
         <v>67</v>
       </c>
@@ -5221,8 +7543,12 @@
       <c r="E74">
         <v>1.6539999999999999</v>
       </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F74">
+        <f t="shared" si="1"/>
+        <v>-0.23299999999999987</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A75">
         <v>68</v>
       </c>
@@ -5238,8 +7564,12 @@
       <c r="E75">
         <v>1.653</v>
       </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F75">
+        <f t="shared" si="1"/>
+        <v>-0.23799999999999999</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A76">
         <v>69</v>
       </c>
@@ -5255,8 +7585,12 @@
       <c r="E76">
         <v>1.633</v>
       </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F76">
+        <f t="shared" si="1"/>
+        <v>-0.21999999999999997</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A77">
         <v>70</v>
       </c>
@@ -5272,8 +7606,12 @@
       <c r="E77">
         <v>1.6240000000000001</v>
       </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F77">
+        <f t="shared" si="1"/>
+        <v>-0.22300000000000009</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A78">
         <v>71</v>
       </c>
@@ -5289,8 +7627,12 @@
       <c r="E78">
         <v>1.621</v>
       </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F78">
+        <f t="shared" si="1"/>
+        <v>-0.21100000000000008</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A79">
         <v>72</v>
       </c>
@@ -5306,8 +7648,12 @@
       <c r="E79">
         <v>1.611</v>
       </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F79">
+        <f t="shared" si="1"/>
+        <v>-0.20500000000000007</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A80">
         <v>73</v>
       </c>
@@ -5323,229 +7669,1137 @@
       <c r="E80">
         <v>1.603</v>
       </c>
-    </row>
-    <row r="81" spans="4:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F80">
+        <f t="shared" si="1"/>
+        <v>-0.20300000000000007</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A81">
+        <v>74</v>
+      </c>
+      <c r="B81">
+        <v>1.391</v>
+      </c>
       <c r="D81">
         <v>71</v>
       </c>
       <c r="E81">
         <v>1.603</v>
       </c>
-    </row>
-    <row r="82" spans="4:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F81">
+        <f t="shared" si="1"/>
+        <v>-0.21199999999999997</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A82">
+        <v>75</v>
+      </c>
+      <c r="B82">
+        <v>1.389</v>
+      </c>
       <c r="D82">
         <v>72</v>
       </c>
       <c r="E82">
         <v>1.5880000000000001</v>
       </c>
-    </row>
-    <row r="83" spans="4:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F82">
+        <f t="shared" si="1"/>
+        <v>-0.19900000000000007</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A83">
+        <v>76</v>
+      </c>
+      <c r="B83">
+        <v>1.391</v>
+      </c>
       <c r="D83">
         <v>73</v>
       </c>
       <c r="E83">
         <v>1.577</v>
       </c>
-    </row>
-    <row r="84" spans="4:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F83">
+        <f t="shared" si="1"/>
+        <v>-0.18599999999999994</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A84">
+        <v>77</v>
+      </c>
+      <c r="B84">
+        <v>1.38</v>
+      </c>
       <c r="D84">
         <v>74</v>
       </c>
       <c r="E84">
         <v>1.57</v>
       </c>
-    </row>
-    <row r="85" spans="4:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F84">
+        <f t="shared" si="1"/>
+        <v>-0.19000000000000017</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A85">
+        <v>78</v>
+      </c>
+      <c r="B85">
+        <v>1.3720000000000001</v>
+      </c>
       <c r="D85">
         <v>75</v>
       </c>
       <c r="E85">
         <v>1.569</v>
       </c>
-    </row>
-    <row r="86" spans="4:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F85">
+        <f t="shared" si="1"/>
+        <v>-0.19699999999999984</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A86">
+        <v>79</v>
+      </c>
+      <c r="B86">
+        <v>1.3660000000000001</v>
+      </c>
       <c r="D86">
         <v>76</v>
       </c>
       <c r="E86">
         <v>1.556</v>
       </c>
-    </row>
-    <row r="87" spans="4:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F86">
+        <f t="shared" si="1"/>
+        <v>-0.18999999999999995</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A87">
+        <v>80</v>
+      </c>
+      <c r="B87">
+        <v>1.369</v>
+      </c>
       <c r="D87">
         <v>77</v>
       </c>
       <c r="E87">
         <v>1.5449999999999999</v>
       </c>
-    </row>
-    <row r="88" spans="4:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F87">
+        <f t="shared" si="1"/>
+        <v>-0.17599999999999993</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A88">
+        <v>81</v>
+      </c>
+      <c r="B88">
+        <v>1.367</v>
+      </c>
       <c r="D88">
         <v>78</v>
       </c>
       <c r="E88">
         <v>1.5389999999999999</v>
       </c>
-    </row>
-    <row r="89" spans="4:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F88">
+        <f t="shared" si="1"/>
+        <v>-0.17199999999999993</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A89">
+        <v>82</v>
+      </c>
+      <c r="B89">
+        <v>1.3540000000000001</v>
+      </c>
       <c r="D89">
         <v>79</v>
       </c>
       <c r="E89">
         <v>1.5349999999999999</v>
       </c>
-    </row>
-    <row r="90" spans="4:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F89">
+        <f t="shared" si="1"/>
+        <v>-0.18099999999999983</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A90">
+        <v>83</v>
+      </c>
+      <c r="B90">
+        <v>1.3560000000000001</v>
+      </c>
       <c r="D90">
         <v>80</v>
       </c>
       <c r="E90">
         <v>1.5249999999999999</v>
       </c>
-    </row>
-    <row r="91" spans="4:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F90">
+        <f t="shared" si="1"/>
+        <v>-0.16899999999999982</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A91">
+        <v>84</v>
+      </c>
+      <c r="B91">
+        <v>1.351</v>
+      </c>
       <c r="D91">
         <v>81</v>
       </c>
       <c r="E91">
         <v>1.5189999999999999</v>
       </c>
-    </row>
-    <row r="92" spans="4:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F91">
+        <f t="shared" si="1"/>
+        <v>-0.16799999999999993</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A92">
+        <v>85</v>
+      </c>
+      <c r="B92">
+        <v>1.3480000000000001</v>
+      </c>
       <c r="D92">
         <v>82</v>
       </c>
       <c r="E92">
         <v>1.514</v>
       </c>
-    </row>
-    <row r="93" spans="4:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F92">
+        <f t="shared" si="1"/>
+        <v>-0.16599999999999993</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A93">
+        <v>86</v>
+      </c>
+      <c r="B93">
+        <v>1.347</v>
+      </c>
       <c r="D93">
         <v>83</v>
       </c>
       <c r="E93">
         <v>1.512</v>
       </c>
-    </row>
-    <row r="94" spans="4:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F93">
+        <f t="shared" si="1"/>
+        <v>-0.16500000000000004</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A94">
+        <v>87</v>
+      </c>
+      <c r="B94">
+        <v>1.347</v>
+      </c>
       <c r="D94">
         <v>84</v>
       </c>
       <c r="E94">
         <v>1.502</v>
       </c>
-    </row>
-    <row r="95" spans="4:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F94">
+        <f t="shared" si="1"/>
+        <v>-0.15500000000000003</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A95">
+        <v>88</v>
+      </c>
+      <c r="B95">
+        <v>1.3380000000000001</v>
+      </c>
       <c r="D95">
         <v>85</v>
       </c>
       <c r="E95">
         <v>1.5049999999999999</v>
       </c>
-    </row>
-    <row r="96" spans="4:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F95">
+        <f t="shared" si="1"/>
+        <v>-0.16699999999999982</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A96">
+        <v>89</v>
+      </c>
+      <c r="B96">
+        <v>1.333</v>
+      </c>
       <c r="D96">
         <v>86</v>
       </c>
       <c r="E96">
         <v>1.4930000000000001</v>
       </c>
-    </row>
-    <row r="97" spans="4:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F96">
+        <f t="shared" si="1"/>
+        <v>-0.16000000000000014</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A97">
+        <v>90</v>
+      </c>
+      <c r="B97">
+        <v>1.3360000000000001</v>
+      </c>
       <c r="D97">
         <v>87</v>
       </c>
       <c r="E97">
         <v>1.478</v>
       </c>
-    </row>
-    <row r="98" spans="4:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F97">
+        <f t="shared" si="1"/>
+        <v>-0.1419999999999999</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A98">
+        <v>91</v>
+      </c>
+      <c r="B98">
+        <v>1.335</v>
+      </c>
       <c r="D98">
         <v>88</v>
       </c>
       <c r="E98">
         <v>1.48</v>
       </c>
-    </row>
-    <row r="99" spans="4:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F98">
+        <f t="shared" si="1"/>
+        <v>-0.14500000000000002</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A99">
+        <v>92</v>
+      </c>
+      <c r="B99">
+        <v>1.331</v>
+      </c>
       <c r="D99">
         <v>89</v>
       </c>
       <c r="E99">
         <v>1.478</v>
       </c>
-    </row>
-    <row r="100" spans="4:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F99">
+        <f t="shared" si="1"/>
+        <v>-0.14700000000000002</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A100">
+        <v>93</v>
+      </c>
+      <c r="B100">
+        <v>1.3260000000000001</v>
+      </c>
       <c r="D100">
         <v>90</v>
       </c>
       <c r="E100">
         <v>1.4690000000000001</v>
       </c>
-    </row>
-    <row r="101" spans="4:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F100">
+        <f t="shared" si="1"/>
+        <v>-0.14300000000000002</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A101">
+        <v>94</v>
+      </c>
+      <c r="B101">
+        <v>1.3220000000000001</v>
+      </c>
       <c r="D101">
         <v>91</v>
       </c>
       <c r="E101">
         <v>1.4650000000000001</v>
       </c>
-    </row>
-    <row r="102" spans="4:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F101">
+        <f t="shared" si="1"/>
+        <v>-0.14300000000000002</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A102">
+        <v>95</v>
+      </c>
+      <c r="B102">
+        <v>1.323</v>
+      </c>
       <c r="D102">
         <v>92</v>
       </c>
       <c r="E102">
         <v>1.4610000000000001</v>
       </c>
-    </row>
-    <row r="103" spans="4:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F102">
+        <f t="shared" si="1"/>
+        <v>-0.13800000000000012</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A103">
+        <f>A102+1</f>
+        <v>96</v>
+      </c>
+      <c r="B103">
+        <v>1.3169999999999999</v>
+      </c>
       <c r="D103">
         <v>93</v>
       </c>
       <c r="E103">
         <v>1.454</v>
       </c>
-    </row>
-    <row r="104" spans="4:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F103">
+        <f t="shared" si="1"/>
+        <v>-0.13700000000000001</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A104">
+        <f t="shared" ref="A104:A130" si="2">A103+1</f>
+        <v>97</v>
+      </c>
+      <c r="B104">
+        <v>1.3140000000000001</v>
+      </c>
       <c r="D104">
         <v>94</v>
       </c>
       <c r="E104">
         <v>1.4510000000000001</v>
       </c>
-    </row>
-    <row r="105" spans="4:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F104">
+        <f t="shared" si="1"/>
+        <v>-0.13700000000000001</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A105">
+        <f t="shared" si="2"/>
+        <v>98</v>
+      </c>
+      <c r="B105">
+        <v>1.3129999999999999</v>
+      </c>
       <c r="D105">
         <v>95</v>
       </c>
       <c r="E105">
         <v>1.4419999999999999</v>
       </c>
-    </row>
-    <row r="106" spans="4:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F105">
+        <f t="shared" si="1"/>
+        <v>-0.129</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A106">
+        <f t="shared" si="2"/>
+        <v>99</v>
+      </c>
+      <c r="B106">
+        <v>1.3140000000000001</v>
+      </c>
       <c r="D106">
         <v>96</v>
       </c>
       <c r="E106">
         <v>1.4359999999999999</v>
       </c>
-    </row>
-    <row r="107" spans="4:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F106">
+        <f t="shared" si="1"/>
+        <v>-0.12199999999999989</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A107">
+        <f t="shared" si="2"/>
+        <v>100</v>
+      </c>
+      <c r="B107">
+        <v>1.3049999999999999</v>
+      </c>
       <c r="D107">
         <v>97</v>
       </c>
       <c r="E107">
         <v>1.4359999999999999</v>
       </c>
-    </row>
-    <row r="108" spans="4:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F107">
+        <f t="shared" si="1"/>
+        <v>-0.13100000000000001</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A108">
+        <f t="shared" si="2"/>
+        <v>101</v>
+      </c>
+      <c r="B108">
+        <v>1.3</v>
+      </c>
       <c r="D108">
         <v>98</v>
       </c>
       <c r="E108">
         <v>1.431</v>
+      </c>
+      <c r="F108">
+        <f t="shared" si="1"/>
+        <v>-0.13100000000000001</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A109">
+        <f t="shared" si="2"/>
+        <v>102</v>
+      </c>
+      <c r="B109">
+        <v>1.296</v>
+      </c>
+      <c r="D109">
+        <v>111</v>
+      </c>
+      <c r="E109">
+        <v>1.3740000000000001</v>
+      </c>
+      <c r="F109">
+        <f t="shared" si="1"/>
+        <v>-7.8000000000000069E-2</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A110">
+        <f t="shared" si="2"/>
+        <v>103</v>
+      </c>
+      <c r="B110">
+        <v>1.2909999999999999</v>
+      </c>
+      <c r="D110">
+        <v>112</v>
+      </c>
+      <c r="E110">
+        <v>1.3640000000000001</v>
+      </c>
+      <c r="F110">
+        <f t="shared" si="1"/>
+        <v>-7.3000000000000176E-2</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A111">
+        <f t="shared" si="2"/>
+        <v>104</v>
+      </c>
+      <c r="B111">
+        <v>1.298</v>
+      </c>
+      <c r="D111">
+        <v>113</v>
+      </c>
+      <c r="E111">
+        <v>1.369</v>
+      </c>
+      <c r="F111">
+        <f t="shared" si="1"/>
+        <v>-7.0999999999999952E-2</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A112">
+        <f t="shared" si="2"/>
+        <v>105</v>
+      </c>
+      <c r="B112">
+        <v>1.2949999999999999</v>
+      </c>
+      <c r="D112">
+        <v>114</v>
+      </c>
+      <c r="E112">
+        <v>1.357</v>
+      </c>
+      <c r="F112">
+        <f t="shared" si="1"/>
+        <v>-6.2000000000000055E-2</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A113">
+        <f t="shared" si="2"/>
+        <v>106</v>
+      </c>
+      <c r="B113">
+        <v>1.2909999999999999</v>
+      </c>
+      <c r="D113">
+        <v>115</v>
+      </c>
+      <c r="E113">
+        <v>1.355</v>
+      </c>
+      <c r="F113">
+        <f t="shared" si="1"/>
+        <v>-6.4000000000000057E-2</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A114">
+        <f t="shared" si="2"/>
+        <v>107</v>
+      </c>
+      <c r="B114">
+        <v>1.2849999999999999</v>
+      </c>
+      <c r="D114">
+        <v>116</v>
+      </c>
+      <c r="E114">
+        <v>1.355</v>
+      </c>
+      <c r="F114">
+        <f t="shared" si="1"/>
+        <v>-7.0000000000000062E-2</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A115">
+        <f t="shared" si="2"/>
+        <v>108</v>
+      </c>
+      <c r="B115">
+        <v>1.284</v>
+      </c>
+      <c r="D115">
+        <v>117</v>
+      </c>
+      <c r="E115">
+        <v>1.3540000000000001</v>
+      </c>
+      <c r="F115">
+        <f t="shared" si="1"/>
+        <v>-7.0000000000000062E-2</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A116">
+        <f t="shared" si="2"/>
+        <v>109</v>
+      </c>
+      <c r="B116">
+        <v>1.2849999999999999</v>
+      </c>
+      <c r="D116">
+        <v>118</v>
+      </c>
+      <c r="E116">
+        <v>1.3480000000000001</v>
+      </c>
+      <c r="F116">
+        <f t="shared" si="1"/>
+        <v>-6.3000000000000167E-2</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A117">
+        <f t="shared" si="2"/>
+        <v>110</v>
+      </c>
+      <c r="B117">
+        <v>1.274</v>
+      </c>
+      <c r="D117">
+        <v>119</v>
+      </c>
+      <c r="E117">
+        <v>1.343</v>
+      </c>
+      <c r="F117">
+        <f t="shared" si="1"/>
+        <v>-6.899999999999995E-2</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A118">
+        <f t="shared" si="2"/>
+        <v>111</v>
+      </c>
+      <c r="B118">
+        <v>1.2789999999999999</v>
+      </c>
+      <c r="D118">
+        <v>120</v>
+      </c>
+      <c r="E118">
+        <v>1.347</v>
+      </c>
+      <c r="F118">
+        <f t="shared" si="1"/>
+        <v>-6.800000000000006E-2</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A119">
+        <f t="shared" si="2"/>
+        <v>112</v>
+      </c>
+      <c r="B119">
+        <v>1.2789999999999999</v>
+      </c>
+      <c r="D119">
+        <v>121</v>
+      </c>
+      <c r="E119">
+        <v>1.335</v>
+      </c>
+      <c r="F119">
+        <f t="shared" si="1"/>
+        <v>-5.600000000000005E-2</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A120">
+        <f t="shared" si="2"/>
+        <v>113</v>
+      </c>
+      <c r="B120">
+        <v>1.2769999999999999</v>
+      </c>
+      <c r="D120">
+        <v>122</v>
+      </c>
+      <c r="E120">
+        <v>1.3420000000000001</v>
+      </c>
+      <c r="F120">
+        <f t="shared" si="1"/>
+        <v>-6.5000000000000169E-2</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A121">
+        <f t="shared" si="2"/>
+        <v>114</v>
+      </c>
+      <c r="B121">
+        <v>1.27</v>
+      </c>
+      <c r="D121">
+        <v>123</v>
+      </c>
+      <c r="E121">
+        <v>1.3340000000000001</v>
+      </c>
+      <c r="F121">
+        <f t="shared" si="1"/>
+        <v>-6.4000000000000057E-2</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A122">
+        <f t="shared" si="2"/>
+        <v>115</v>
+      </c>
+      <c r="B122">
+        <v>1.272</v>
+      </c>
+      <c r="D122">
+        <v>124</v>
+      </c>
+      <c r="E122">
+        <v>1.3280000000000001</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A123">
+        <f t="shared" si="2"/>
+        <v>116</v>
+      </c>
+      <c r="D123">
+        <v>125</v>
+      </c>
+      <c r="E123">
+        <v>1.33</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A124">
+        <f t="shared" si="2"/>
+        <v>117</v>
+      </c>
+      <c r="D124">
+        <v>126</v>
+      </c>
+      <c r="E124">
+        <v>1.323</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A125">
+        <f t="shared" si="2"/>
+        <v>118</v>
+      </c>
+      <c r="D125">
+        <v>127</v>
+      </c>
+      <c r="E125">
+        <v>1.32</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A126">
+        <f t="shared" si="2"/>
+        <v>119</v>
+      </c>
+      <c r="D126">
+        <v>128</v>
+      </c>
+      <c r="E126">
+        <v>1.323</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A127">
+        <f t="shared" si="2"/>
+        <v>120</v>
+      </c>
+      <c r="D127">
+        <v>129</v>
+      </c>
+      <c r="E127">
+        <v>1.3169999999999999</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A128">
+        <f t="shared" si="2"/>
+        <v>121</v>
+      </c>
+      <c r="D128">
+        <v>130</v>
+      </c>
+      <c r="E128">
+        <v>1.3120000000000001</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A129">
+        <f t="shared" si="2"/>
+        <v>122</v>
+      </c>
+      <c r="D129">
+        <v>131</v>
+      </c>
+      <c r="E129">
+        <v>1.3089999999999999</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A130">
+        <f t="shared" si="2"/>
+        <v>123</v>
+      </c>
+      <c r="D130">
+        <v>132</v>
+      </c>
+      <c r="E130">
+        <v>1.306</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="D131">
+        <v>133</v>
+      </c>
+      <c r="E131">
+        <v>1.298</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="D132">
+        <f>D131+1</f>
+        <v>134</v>
+      </c>
+      <c r="E132">
+        <v>1.304</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="D133">
+        <f t="shared" ref="D133:D160" si="3">D132+1</f>
+        <v>135</v>
+      </c>
+      <c r="E133">
+        <v>1.2949999999999999</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="D134">
+        <f t="shared" si="3"/>
+        <v>136</v>
+      </c>
+      <c r="E134">
+        <v>1.302</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="D135">
+        <f t="shared" si="3"/>
+        <v>137</v>
+      </c>
+      <c r="E135">
+        <v>1.298</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="D136">
+        <f t="shared" si="3"/>
+        <v>138</v>
+      </c>
+      <c r="E136">
+        <v>1.2969999999999999</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="D137">
+        <f t="shared" si="3"/>
+        <v>139</v>
+      </c>
+      <c r="E137">
+        <v>1.2929999999999999</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="D138">
+        <f t="shared" si="3"/>
+        <v>140</v>
+      </c>
+      <c r="E138">
+        <v>1.282</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="D139">
+        <f t="shared" si="3"/>
+        <v>141</v>
+      </c>
+      <c r="E139">
+        <v>1.2809999999999999</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="D140">
+        <f t="shared" si="3"/>
+        <v>142</v>
+      </c>
+      <c r="E140">
+        <v>1.2849999999999999</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="D141">
+        <f t="shared" si="3"/>
+        <v>143</v>
+      </c>
+      <c r="E141">
+        <v>1.282</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="D142">
+        <f t="shared" si="3"/>
+        <v>144</v>
+      </c>
+      <c r="E142">
+        <v>1.2789999999999999</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="D143">
+        <f t="shared" si="3"/>
+        <v>145</v>
+      </c>
+      <c r="E143">
+        <v>1.2649999999999999</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="D144">
+        <f t="shared" si="3"/>
+        <v>146</v>
+      </c>
+      <c r="E144">
+        <v>1.268</v>
+      </c>
+    </row>
+    <row r="145" spans="4:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="D145">
+        <f t="shared" si="3"/>
+        <v>147</v>
+      </c>
+      <c r="E145">
+        <v>1.2709999999999999</v>
+      </c>
+    </row>
+    <row r="146" spans="4:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="D146">
+        <f t="shared" si="3"/>
+        <v>148</v>
+      </c>
+      <c r="E146">
+        <v>1.27</v>
+      </c>
+    </row>
+    <row r="147" spans="4:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="D147">
+        <f t="shared" si="3"/>
+        <v>149</v>
+      </c>
+      <c r="E147">
+        <v>1.2649999999999999</v>
+      </c>
+    </row>
+    <row r="148" spans="4:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="D148">
+        <f t="shared" si="3"/>
+        <v>150</v>
+      </c>
+      <c r="E148">
+        <v>1.27</v>
+      </c>
+    </row>
+    <row r="149" spans="4:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="D149">
+        <f t="shared" si="3"/>
+        <v>151</v>
+      </c>
+      <c r="E149">
+        <v>1.2629999999999999</v>
+      </c>
+    </row>
+    <row r="150" spans="4:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="D150">
+        <f t="shared" si="3"/>
+        <v>152</v>
+      </c>
+      <c r="E150">
+        <v>1.262</v>
+      </c>
+    </row>
+    <row r="151" spans="4:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="D151">
+        <f t="shared" si="3"/>
+        <v>153</v>
+      </c>
+      <c r="E151">
+        <v>1.254</v>
+      </c>
+    </row>
+    <row r="152" spans="4:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="D152">
+        <f t="shared" si="3"/>
+        <v>154</v>
+      </c>
+      <c r="E152">
+        <v>1.2509999999999999</v>
+      </c>
+    </row>
+    <row r="153" spans="4:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="D153">
+        <f t="shared" si="3"/>
+        <v>155</v>
+      </c>
+      <c r="E153">
+        <v>1.254</v>
+      </c>
+    </row>
+    <row r="154" spans="4:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="D154">
+        <f t="shared" si="3"/>
+        <v>156</v>
+      </c>
+      <c r="E154">
+        <v>1.254</v>
+      </c>
+    </row>
+    <row r="155" spans="4:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="D155">
+        <f t="shared" si="3"/>
+        <v>157</v>
+      </c>
+      <c r="E155">
+        <v>1.2490000000000001</v>
+      </c>
+    </row>
+    <row r="156" spans="4:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="D156">
+        <f>D155+1</f>
+        <v>158</v>
+      </c>
+      <c r="E156">
+        <v>1.246</v>
+      </c>
+    </row>
+    <row r="157" spans="4:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="D157">
+        <f t="shared" si="3"/>
+        <v>159</v>
+      </c>
+      <c r="E157">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="158" spans="4:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="D158">
+        <f t="shared" si="3"/>
+        <v>160</v>
+      </c>
+    </row>
+    <row r="159" spans="4:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="D159">
+        <f t="shared" si="3"/>
+        <v>161</v>
+      </c>
+    </row>
+    <row r="160" spans="4:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="D160">
+        <f t="shared" si="3"/>
+        <v>162</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
small bug in print
</commit_message>
<xml_diff>
--- a/chatbotp3r3/eloss3and4levelNet.xlsx
+++ b/chatbotp3r3/eloss3and4levelNet.xlsx
@@ -4814,6 +4814,9 @@
                 </c:pt>
                 <c:pt idx="47">
                   <c:v>0.83499999999999996</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.83199999999999996</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7677,8 +7680,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J160"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J51" sqref="J51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -9086,6 +9089,9 @@
       </c>
       <c r="G50">
         <v>1.0009999999999999</v>
+      </c>
+      <c r="J50">
+        <v>0.83199999999999996</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.55000000000000004">

</xml_diff>